<commit_message>
Complete Fruit Project Without Issues
This is an Attended Process Where User interventions required.
</commit_message>
<xml_diff>
--- a/vajrang/Team5/AmazonExtractInfo/Data/Input/amazon excel usecase.xlsx
+++ b/vajrang/Team5/AmazonExtractInfo/Data/Input/amazon excel usecase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uipath Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RPA-Developer-in-30-Days\vajrang\Team5\AmazonExtractInfo\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -167,10 +167,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,14 +201,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,7 +527,7 @@
   <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +874,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +933,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +948,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
@@ -945,6 +956,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete ReframeWork Fruit Project In Attended Mode (#289)
* First Commit

This is the code for sorting the files in there respective Folders (e,g moving excel files to excel folder and pdf files to Pdf folder and so on..)

* Calculator

* Fruit_Project_Task Capture

* Complete Fruit Project Without Issues

This is an Attended Process Where User interventions required.
</commit_message>
<xml_diff>
--- a/vajrang/Team5/AmazonExtractInfo/Data/Input/amazon excel usecase.xlsx
+++ b/vajrang/Team5/AmazonExtractInfo/Data/Input/amazon excel usecase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uipath Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RPA-Developer-in-30-Days\vajrang\Team5\AmazonExtractInfo\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -167,10 +167,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,14 +201,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,7 +527,7 @@
   <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +874,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +933,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +948,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
@@ -945,6 +956,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>